<commit_message>
random dan phim chuyen nghiep
</commit_message>
<xml_diff>
--- a/Last_Bugs/cungphimjobs.xlsx
+++ b/Last_Bugs/cungphimjobs.xlsx
@@ -183,9 +183,6 @@
     <t>Thay doi noi dung : $Co Phieu | @username</t>
   </si>
   <si>
-    <t>Tam thoi load hinh</t>
-  </si>
-  <si>
     <t>Cat gia</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>Thuat toán search</t>
+  </si>
+  <si>
+    <t>Tam thoi load pdf</t>
   </si>
 </sst>
 </file>
@@ -350,7 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -435,9 +435,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,6 +448,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -754,7 +761,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -786,10 +793,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="25" customFormat="1">
@@ -803,7 +810,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="29" customFormat="1">
@@ -817,7 +824,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="29" customFormat="1">
@@ -834,7 +841,7 @@
         <v>33</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>34</v>
@@ -851,7 +858,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>34</v>
@@ -871,7 +878,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="29" customFormat="1">
@@ -885,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>34</v>
@@ -901,8 +908,8 @@
       <c r="C9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="39" t="s">
-        <v>55</v>
+      <c r="E9" s="38" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="17" customFormat="1" ht="30">
@@ -919,7 +926,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="17" customFormat="1">
@@ -933,7 +940,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="33" customFormat="1">
@@ -964,29 +971,29 @@
         <v>2</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="33" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A14" s="30">
+    <row r="14" spans="1:7" s="17" customFormat="1" ht="29.25" customHeight="1">
+      <c r="A14" s="13">
         <v>13</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="33" t="s">
+      <c r="C14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="33" t="s">
+      <c r="F14" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="17" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1023,7 +1030,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" s="33" t="s">
         <v>40</v>
@@ -1043,24 +1050,24 @@
         <v>39</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="12" customFormat="1">
-      <c r="A19" s="35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="42" customFormat="1">
+      <c r="A19" s="39">
         <v>18</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="C19" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="12" t="s">
-        <v>58</v>
+      <c r="F19" s="42" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="17" customFormat="1">
@@ -1075,7 +1082,7 @@
         <v>22</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="29" customFormat="1">
@@ -1087,25 +1094,25 @@
       </c>
       <c r="C21" s="26"/>
       <c r="E21" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="12" customFormat="1">
-      <c r="A22" s="35">
+      <c r="A22" s="34">
         <v>23</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="35"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="17" customFormat="1">
@@ -1120,7 +1127,7 @@
         <v>27</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="17" customFormat="1">
@@ -1136,20 +1143,20 @@
       </c>
     </row>
     <row r="25" spans="1:7" s="12" customFormat="1">
-      <c r="A25" s="35">
+      <c r="A25" s="34">
         <v>26</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="36" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1161,7 +1168,7 @@
       <c r="A27" s="13">
         <v>27</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="37" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="13"/>
@@ -1169,7 +1176,7 @@
         <v>31</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="29" customFormat="1">
@@ -1179,17 +1186,17 @@
       </c>
       <c r="C28" s="26"/>
       <c r="E28" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="17" customFormat="1">
       <c r="A29" s="13"/>
       <c r="B29" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" s="13"/>
       <c r="E29" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>